<commit_message>
minor changes in results (rep2 run2 stereoscope)
</commit_message>
<xml_diff>
--- a/results/summary files/rep2_run2/all_results.xlsx
+++ b/results/summary files/rep2_run2/all_results.xlsx
@@ -820,7 +820,7 @@
         <v>0.9915675432999627</v>
       </c>
       <c r="F39" t="n">
-        <v>0.6576908933130634</v>
+        <v>0.7263647249527185</v>
       </c>
     </row>
     <row r="40">
@@ -840,7 +840,7 @@
         <v>0.0185123090718056</v>
       </c>
       <c r="F40" t="n">
-        <v>0.15292999450148195</v>
+        <v>0.14083773701075356</v>
       </c>
     </row>
     <row r="41">
@@ -860,7 +860,7 @@
         <v>0.92</v>
       </c>
       <c r="F41" t="n">
-        <v>0.62</v>
+        <v>0.63</v>
       </c>
     </row>
     <row r="42">
@@ -900,7 +900,7 @@
         <v>0.91</v>
       </c>
       <c r="F43" t="n">
-        <v>0.58</v>
+        <v>0.59</v>
       </c>
     </row>
     <row r="44">
@@ -920,7 +920,7 @@
         <v>0.57</v>
       </c>
       <c r="F44" t="n">
-        <v>0.21</v>
+        <v>0.22</v>
       </c>
     </row>
     <row r="45">
@@ -940,7 +940,7 @@
         <v>0.73</v>
       </c>
       <c r="F45" t="n">
-        <v>0.35</v>
+        <v>0.36</v>
       </c>
     </row>
     <row r="46">

</xml_diff>